<commit_message>
Day_3 assingnment 2nd commit
</commit_message>
<xml_diff>
--- a/assignments/29Nov/Input/Bank_Reports.xlsx
+++ b/assignments/29Nov/Input/Bank_Reports.xlsx
@@ -10,6 +10,7 @@
     <x:sheet name="June Report" sheetId="2" r:id="rId1"/>
     <x:sheet name="July Report" sheetId="1" r:id="rId2"/>
     <x:sheet name="June Total " sheetId="6" r:id="rId6"/>
+    <x:sheet name="June Total new " sheetId="7" r:id="rId7"/>
   </x:sheets>
   <x:definedNames/>
   <x:calcPr calcId="162913"/>
@@ -337,6 +338,15 @@
   </x:si>
   <x:si>
     <x:t>59661</x:t>
+  </x:si>
+  <x:si>
+    <x:t>235004</x:t>
+  </x:si>
+  <x:si>
+    <x:t>179809</x:t>
+  </x:si>
+  <x:si>
+    <x:t>19565</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -1906,6 +1916,9 @@
       <x:c r="D33" s="1">
         <x:v>195</x:v>
       </x:c>
+      <x:c r="E33" s="0"/>
+      <x:c r="F33" s="0"/>
+      <x:c r="G33" s="0"/>
       <x:c r="H33" s="0"/>
     </x:row>
     <x:row r="34" spans="1:8" x14ac:dyDescent="0.3">
@@ -2595,4 +2608,46 @@
   <x:headerFooter/>
   <x:tableParts count="0"/>
 </x:worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <x:sheetPr>
+    <x:outlinePr summaryBelow="1" summaryRight="1"/>
+  </x:sheetPr>
+  <x:dimension ref="A1:C3"/>
+  <x:sheetViews>
+    <x:sheetView workbookViewId="0"/>
+  </x:sheetViews>
+  <x:sheetFormatPr defaultRowHeight="15"/>
+  <x:sheetData>
+    <x:row r="1" spans="1:3">
+      <x:c r="A1" s="0" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="B1" s="0" t="s">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="C1" s="0" t="s">
+        <x:v>3</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="3" spans="1:3">
+      <x:c r="A3" s="0" t="s">
+        <x:v>105</x:v>
+      </x:c>
+      <x:c r="B3" s="0" t="s">
+        <x:v>106</x:v>
+      </x:c>
+      <x:c r="C3" s="0" t="s">
+        <x:v>107</x:v>
+      </x:c>
+    </x:row>
+  </x:sheetData>
+  <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
+  <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
+  <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>
+  <x:headerFooter/>
+  <x:tableParts count="0"/>
+</x:worksheet>
 </file>
</xml_diff>